<commit_message>
Other small fixes (we are almost there!)
</commit_message>
<xml_diff>
--- a/Data_Process/Fuel_rack_analysis.xlsx
+++ b/Data_Process/Fuel_rack_analysis.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3600,18 +3600,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="O45" sqref="O45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="2.453125" customWidth="1"/>
-    <col min="14" max="14" width="4.26953125" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.42578125" customWidth="1"/>
+    <col min="14" max="14" width="4.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>22</v>
       </c>
@@ -3630,7 +3630,7 @@
         <v>24.232538802060759</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>21</v>
       </c>
@@ -3661,7 +3661,7 @@
       </c>
       <c r="R2" s="3"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -3705,7 +3705,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -3760,7 +3760,7 @@
         <v>5.4502909938287415E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5">
         <v>0.5</v>
@@ -3813,7 +3813,7 @@
         <v>1.8235960312026711E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6">
         <v>0.75</v>
@@ -3866,7 +3866,7 @@
         <v>3.1169925249016489E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7">
         <v>0.85</v>
@@ -3919,7 +3919,7 @@
         <v>1.9200032134268911E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8">
         <v>1</v>
@@ -3972,7 +3972,7 @@
         <v>1.1985100788781731E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -4027,7 +4027,7 @@
         <v>1.1836159379547111E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10">
         <v>0.5</v>
@@ -4072,7 +4072,7 @@
         <v>0.33883123659342551</v>
       </c>
       <c r="Q10">
-        <f t="shared" ref="Q5:Q23" si="14">$E$2*($G$2+$G$1*C10)/($G$2+$G$1*$C$2)*J10</f>
+        <f t="shared" ref="Q10:Q23" si="14">$E$2*($G$2+$G$1*C10)/($G$2+$G$1*$C$2)*J10</f>
         <v>584.2785594779117</v>
       </c>
       <c r="R10" s="2">
@@ -4080,7 +4080,7 @@
         <v>4.9752052487880552E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11">
         <v>0.75</v>
@@ -4133,7 +4133,7 @@
         <v>1.9509428164668191E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12">
         <v>0.85</v>
@@ -4186,7 +4186,7 @@
         <v>2.3560117363395142E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13">
         <v>1</v>
@@ -4239,7 +4239,7 @@
         <v>8.9477298086000825E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>10</v>
       </c>
@@ -4294,7 +4294,7 @@
         <v>2.8625261294263224E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15">
         <v>0.5</v>
@@ -4347,7 +4347,7 @@
         <v>4.466588042406335E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16">
         <v>0.75</v>
@@ -4400,7 +4400,7 @@
         <v>1.1012718755521586E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17">
         <v>0.85</v>
@@ -4453,7 +4453,7 @@
         <v>1.3543171434373943E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18">
         <v>1</v>
@@ -4506,7 +4506,7 @@
         <v>2.3220486111110716E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>11</v>
       </c>
@@ -4561,7 +4561,7 @@
         <v>1.0187251814796084E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20">
         <v>0.5</v>
@@ -4614,7 +4614,7 @@
         <v>3.1012468925290138E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21">
         <v>0.75</v>
@@ -4667,7 +4667,7 @@
         <v>2.2547173024977871E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22">
         <v>0.85</v>
@@ -4720,7 +4720,7 @@
         <v>3.9451027163148788E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23">
         <v>1</v>
@@ -4773,7 +4773,7 @@
         <v>2.9162088381142617E-2</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>23</v>
       </c>
@@ -4787,7 +4787,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B62">
         <f>INDEX(LINEST($C$4:$C$8,$B$4:$B$8),1)</f>
         <v>32.861189801699716</v>
@@ -4805,7 +4805,7 @@
         <v>29.546742209631734</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B63">
         <f>INDEX(LINEST($C$4:$C$8,$B$4:$B$8),2)</f>
         <v>17.983002832861189</v>
@@ -4832,6 +4832,18 @@
     <mergeCell ref="A19:A23"/>
     <mergeCell ref="O2:P2"/>
   </mergeCells>
+  <conditionalFormatting sqref="R4:R23">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>